<commit_message>
Entered entry with UserId:104
</commit_message>
<xml_diff>
--- a/OrigBookLibrary.xlsx
+++ b/OrigBookLibrary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\programming\softwareEng\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\programming\softwareEng\bulky-book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE0D3DE-4117-4FBD-9938-E6965E214937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C27162-7E4D-4E48-BAC9-F628DB5BF38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A2B74C87-EE24-4496-AB2C-99CCF2945409}"/>
+    <workbookView xWindow="6945" yWindow="2400" windowWidth="15375" windowHeight="7875" xr2:uid="{A2B74C87-EE24-4496-AB2C-99CCF2945409}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>UserId</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>Smith Publishing</t>
+  </si>
+  <si>
+    <t>Agricultural Irrigation</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>435-235-656-232</t>
+  </si>
+  <si>
+    <t>Covenant Uni. Research</t>
+  </si>
+  <si>
+    <t>Covenant University</t>
   </si>
 </sst>
 </file>
@@ -420,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB509AF2-91B0-4F88-99EF-E23419E2D2DD}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +468,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -472,6 +487,29 @@
       </c>
       <c r="G2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>